<commit_message>
Punto 4 e ItemHistory
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\GITPROPIO\Meli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\GITPROPIO\ProbleMeli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C83BBC-FB7B-41E1-8959-A40BD1148189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FDC731-DBEE-4689-9CEA-F333DE4D3E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="4" xr2:uid="{D9AA5833-F3A1-49C3-9E4D-9B9F0B3C3535}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="5" xr2:uid="{D9AA5833-F3A1-49C3-9E4D-9B9F0B3C3535}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Product" sheetId="3" r:id="rId3"/>
     <sheet name="Order" sheetId="5" r:id="rId4"/>
     <sheet name="Item" sheetId="6" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="953">
   <si>
     <t>FirstName</t>
   </si>
@@ -2894,6 +2895,9 @@
   </si>
   <si>
     <t>dateadd(day,rand(checksum(newid()))*(1+datediff(day, @FromDate2, @ToDate2)),@FromDate2)</t>
+  </si>
+  <si>
+    <t>1488700.00</t>
   </si>
 </sst>
 </file>
@@ -2952,7 +2956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -2968,6 +2972,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -3352,7 +3357,7 @@
         <v>308</v>
       </c>
       <c r="H2" s="1" t="str">
-        <f>TEXT(F2,"aaaa-mm-dd")</f>
+        <f t="shared" ref="H2:H33" si="0">TEXT(F2,"aaaa-mm-dd")</f>
         <v>1990-07-13</v>
       </c>
       <c r="I2" t="str">
@@ -3383,11 +3388,11 @@
         <v>80</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f>TEXT(F3,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1994-03-07</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I66" si="0">CONCATENATE("INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (",A3,", '",B3,"','",C3,"','",D3,"','",E3,"','",H3,"','",G3,"',getdate());")</f>
+        <f t="shared" ref="I3:I66" si="1">CONCATENATE("INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (",A3,", '",B3,"','",C3,"','",D3,"','",E3,"','",H3,"','",G3,"',getdate());")</f>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ac.risus@volutpatNulla.ca','Octavio','Saavedra','8949 Dictum Avenue','1994-03-07','16680526 6787',getdate());</v>
       </c>
     </row>
@@ -3414,11 +3419,11 @@
         <v>388</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f>TEXT(F4,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1966-08-23</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'aliquam.arcu.Aliquam@adipiscinglobortis.edu','Emiliano','Fernández','773-1441 Molestie Road','1966-08-23','16150704 6348',getdate());</v>
       </c>
     </row>
@@ -3445,11 +3450,11 @@
         <v>142</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>TEXT(F5,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1982-04-27</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'aliquam.eu.accumsan@euismod.com','Elliot','Herrera','9008 Interdum Rd.','1982-04-27','16091130 5142',getdate());</v>
       </c>
     </row>
@@ -3476,11 +3481,11 @@
         <v>188</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f>TEXT(F6,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1973-10-05</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'aliquet.libero.Integer@ac.org','Matthew','Martínez','P.O. Box 737, 4813 Sit St.','1973-10-05','16140405 4254',getdate());</v>
       </c>
     </row>
@@ -3507,11 +3512,11 @@
         <v>253</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f>TEXT(F7,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1984-03-31</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'aliquet@eratvel.ca','Fabrizzio','Gómez','318-6671 Mus. Street','1984-03-31','16691030 0281',getdate());</v>
       </c>
     </row>
@@ -3538,11 +3543,11 @@
         <v>128</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>TEXT(F8,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>2000-10-17</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'amet.metus.Aliquam@magnaDuisdignissim.org','Henrry','Silva','P.O. Box 795, 3428 Aenean Ave','2000-10-17','16801224 7659',getdate());</v>
       </c>
     </row>
@@ -3569,11 +3574,11 @@
         <v>459</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>TEXT(F9,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1972-02-13</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'amet.ultricies.sem@etipsumcursus.edu','Wilfredo','Saavedra','3218 Sodales Avenue','1972-02-13','16260405 9580',getdate());</v>
       </c>
     </row>
@@ -3600,11 +3605,11 @@
         <v>162</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>TEXT(F10,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1972-10-08</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'amet@Fuscealiquet.co.uk','Emanuel','Gallardo','P.O. Box 400, 491 Nulla. St.','1972-10-08','16810904 8820',getdate());</v>
       </c>
     </row>
@@ -3631,11 +3636,11 @@
         <v>401</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>TEXT(F11,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1975-09-27</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ante.ipsum.primis@sagittissemperNam.net','Maxi','Carrasco','Ap #335-5595 A St.','1975-09-27','16851020 1232',getdate());</v>
       </c>
     </row>
@@ -3662,11 +3667,11 @@
         <v>357</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>TEXT(F12,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1984-03-13</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'at.iaculis.quis@Nulladignissim.org','Eliam','Palma','775-5853 Arcu. St.','1984-03-13','16981111 9610',getdate());</v>
       </c>
     </row>
@@ -3693,11 +3698,11 @@
         <v>338</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>TEXT(F13,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1967-01-06</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'at.lacus@feugiatnec.co.uk','Stefano38','Palma','P.O. Box 591, 7643 Elit Street','1967-01-06','16200101 7785',getdate());</v>
       </c>
     </row>
@@ -3724,11 +3729,11 @@
         <v>369</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>TEXT(F14,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1991-10-19</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'at@consequat.co.uk','Lian','Jiménez','394-545 Vestibulum Rd.','1991-10-19','16111118 5011',getdate());</v>
       </c>
     </row>
@@ -3755,11 +3760,11 @@
         <v>38</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>TEXT(F15,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1973-05-21</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'at@sit.ca','Kenneth','García','Ap #213-6174 Lacus. Rd.','1973-05-21','16410629 5191',getdate());</v>
       </c>
     </row>
@@ -3786,11 +3791,11 @@
         <v>329</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>TEXT(F16,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1961-09-05</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'augue.porttitor.interdum@Donecvitae.ca','Exzequiel','Gallardo','205-5574 Vulputate, Av.','1961-09-05','16080911 1529',getdate());</v>
       </c>
     </row>
@@ -3817,11 +3822,11 @@
         <v>99</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>TEXT(F17,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1993-03-30</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'convallis.ante@imperdieteratnonummy.net','Mateo','Toro','2985 Ut, Ave','1993-03-30','16950811 8677',getdate());</v>
       </c>
     </row>
@@ -3848,11 +3853,11 @@
         <v>348</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>TEXT(F18,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1972-04-08</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Cras.vehicula@egetdictum.ca','Benjamin','Yáñez','9290 Et Av.','1972-04-08','16261218 9726',getdate());</v>
       </c>
     </row>
@@ -3879,11 +3884,11 @@
         <v>263</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>TEXT(F19,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1974-01-19</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Cras.vehicula@enimCurabiturmassa.net','Andriu','Araya','5940 Ac Rd.','1974-01-19','16150401 1782',getdate());</v>
       </c>
     </row>
@@ -3910,11 +3915,11 @@
         <v>276</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>TEXT(F20,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1969-12-12</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Cras.vulputate.velit@Aliquameratvolutpat.co.uk','Gregory','Guzmán','1223 Lectus Ave','1969-12-12','16581101 4785',getdate());</v>
       </c>
     </row>
@@ -3941,11 +3946,11 @@
         <v>216</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>TEXT(F21,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1967-03-24</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'cursus.Nunc.mauris@Cum.org','Axl','Peña','368-3734 Aliquam Rd.','1967-03-24','16580106 7470',getdate());</v>
       </c>
     </row>
@@ -3972,11 +3977,11 @@
         <v>206</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f>TEXT(F22,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1974-03-04</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'cursus@nonduinec.co.uk','Benjamín','Sepúlveda','5871 Neque. St.','1974-03-04','16761014 1579',getdate());</v>
       </c>
     </row>
@@ -4003,11 +4008,11 @@
         <v>392</v>
       </c>
       <c r="H23" s="1" t="str">
-        <f>TEXT(F23,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1993-01-31</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'diam.at.pretium@atlacus.edu','Naim','Venegas','331-1595 Purus. Avenue','1993-01-31','16431004 5952',getdate());</v>
       </c>
     </row>
@@ -4034,11 +4039,11 @@
         <v>75</v>
       </c>
       <c r="H24" s="1" t="str">
-        <f>TEXT(F24,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1966-01-02</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'diam.Proin.dolor@sit.co.uk','Lautaro','Ortiz','797-9462 Phasellus Rd.','1966-01-02','16121227 5034',getdate());</v>
       </c>
     </row>
@@ -4065,11 +4070,11 @@
         <v>374</v>
       </c>
       <c r="H25" s="1" t="str">
-        <f>TEXT(F25,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1987-02-19</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'diam@arcuSed.ca','Jesus','Poblete','6798 At St.','1987-02-19','16800522 7726',getdate());</v>
       </c>
     </row>
@@ -4096,11 +4101,11 @@
         <v>41</v>
       </c>
       <c r="H26" s="1" t="str">
-        <f>TEXT(F26,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1966-09-07</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'dignissim.Maecenas@arcuVivamus.edu','Kenneth','Fuentes','894-1366 A Av.','1966-09-07','16210206 9339',getdate());</v>
       </c>
     </row>
@@ -4127,11 +4132,11 @@
         <v>437</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f>TEXT(F27,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>2001-07-17</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'dolor.Quisque.tincidunt@tellussem.co.uk','Julio','Cárdenas','9527 Fusce Av.','2001-07-17','16320409 6436',getdate());</v>
       </c>
     </row>
@@ -4158,11 +4163,11 @@
         <v>272</v>
       </c>
       <c r="H28" s="1" t="str">
-        <f>TEXT(F28,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1993-08-29</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Donec.elementum.lorem@semmagna.org','Mario','Vidal','407-1615 Ornare, Rd.','1993-08-29','16621208 6646',getdate());</v>
       </c>
     </row>
@@ -4189,11 +4194,11 @@
         <v>66</v>
       </c>
       <c r="H29" s="1" t="str">
-        <f>TEXT(F29,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1998-08-17</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Duis.volutpat@sedtortor.co.uk','Maicol','Olivares','P.O. Box 353, 6758 Metus. Rd.','1998-08-17','16260421 7196',getdate());</v>
       </c>
     </row>
@@ -4220,11 +4225,11 @@
         <v>325</v>
       </c>
       <c r="H30" s="1" t="str">
-        <f>TEXT(F30,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1996-09-13</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'eget@diamloremauctor.ca','Isaías','Bustos','P.O. Box 590, 7401 Ut Rd.','1996-09-13','16920109 3128',getdate());</v>
       </c>
     </row>
@@ -4251,11 +4256,11 @@
         <v>463</v>
       </c>
       <c r="H31" s="1" t="str">
-        <f>TEXT(F31,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1975-08-22</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'elementum.at.egestas@acfermentumvel.net','Marck','Jiménez','P.O. Box 921, 2645 Enim. St.','1975-08-22','16070404 6804',getdate());</v>
       </c>
     </row>
@@ -4282,11 +4287,11 @@
         <v>290</v>
       </c>
       <c r="H32" s="1" t="str">
-        <f>TEXT(F32,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1960-10-27</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'elit@felisadipiscingfringilla.ca','Goran','Aravena','2720 Arcu. Rd.','1960-10-27','16000101 1824',getdate());</v>
       </c>
     </row>
@@ -4313,11 +4318,11 @@
         <v>171</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f>TEXT(F33,"aaaa-mm-dd")</f>
+        <f t="shared" si="0"/>
         <v>1993-02-13</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'enim@justoProinnon.org','Deivid','Ruiz','461-9674 Eros Ave','1993-02-13','16130609 0067',getdate());</v>
       </c>
     </row>
@@ -4344,11 +4349,11 @@
         <v>433</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f>TEXT(F34,"aaaa-mm-dd")</f>
+        <f t="shared" ref="H34:H65" si="2">TEXT(F34,"aaaa-mm-dd")</f>
         <v>1960-07-20</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'eros@mauris.ca','Mattias','Rodríguez','992-3450 Velit St.','1960-07-20','16030919 8638',getdate());</v>
       </c>
     </row>
@@ -4375,11 +4380,11 @@
         <v>180</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f>TEXT(F35,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1980-04-04</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'eros@tempusmauriserat.ca','Geremías','Bravo','P.O. Box 316, 3395 Elit, Road','1980-04-04','16931106 7210',getdate());</v>
       </c>
     </row>
@@ -4406,11 +4411,11 @@
         <v>313</v>
       </c>
       <c r="H36" s="1" t="str">
-        <f>TEXT(F36,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1971-05-22</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'est@etrutrumeu.co.uk','Maikol','Cárdenas','P.O. Box 352, 184 Tortor, St.','1971-05-22','16340308 2534',getdate());</v>
       </c>
     </row>
@@ -4437,11 +4442,11 @@
         <v>396</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f>TEXT(F37,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1994-03-19</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'eu.arcu.Morbi@dui.net','Vincent','Cáceres','P.O. Box 218, 2231 Scelerisque St.','1994-03-19','16290301 8535',getdate());</v>
       </c>
     </row>
@@ -4468,11 +4473,11 @@
         <v>90</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f>TEXT(F38,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1969-07-07</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'eu.nibh.vulputate@nisi.edu','Andrés','Toro','P.O. Box 635, 209 Dignissim St.','1969-07-07','16571014 8007',getdate());</v>
       </c>
     </row>
@@ -4499,11 +4504,11 @@
         <v>361</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f>TEXT(F39,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1999-02-16</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'eu.sem@eu.co.uk','Eluney','Gallardo','798-6994 Vel Street','1999-02-16','16250315 7923',getdate());</v>
       </c>
     </row>
@@ -4530,11 +4535,11 @@
         <v>23</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f>TEXT(F40,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1988-07-04</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'fames.ac.turpis@consequatnec.co.uk','Mitchell','Riquelme','P.O. Box 670, 9786 Dictum Rd.','1988-07-04','16031223 0436',getdate());</v>
       </c>
     </row>
@@ -4561,11 +4566,11 @@
         <v>383</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f>TEXT(F41,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1984-07-13</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'felis@Mauris.edu','Joan','Jiménez','3908 Integer Av.','1984-07-13','16421104 8196',getdate());</v>
       </c>
     </row>
@@ -4592,11 +4597,11 @@
         <v>184</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f>TEXT(F42,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>2000-06-07</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'fringilla.cursus.purus@nequenonquam.co.uk','Milton','Ortiz','Ap #500-5734 Donec Rd.','2000-06-07','16030629 7482',getdate());</v>
       </c>
     </row>
@@ -4623,11 +4628,11 @@
         <v>198</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f>TEXT(F43,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1960-03-03</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Fusce.diam@fermentum.org','Angel','Ortega','520-3427 Imperdiet Rd.','1960-03-03','16700813 2396',getdate());</v>
       </c>
     </row>
@@ -4654,11 +4659,11 @@
         <v>133</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f>TEXT(F44,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1994-12-22</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'gravida@Aenean.edu','Arthur','Venegas','Ap #423-9238 Interdum. Ave','1994-12-22','16370113 7832',getdate());</v>
       </c>
     </row>
@@ -4685,11 +4690,11 @@
         <v>147</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f>TEXT(F45,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1960-07-23</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'id.libero.Donec@aclibero.com','Ian','Vargas','P.O. Box 640, 5817 Pede. Street','1960-07-23','16320617 2300',getdate());</v>
       </c>
     </row>
@@ -4716,11 +4721,11 @@
         <v>365</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f>TEXT(F46,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1961-01-08</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'imperdiet.nec@Pellentesque.org','Cristiàn','Olivares','200-3153 Eget, Street','1961-01-08','16880515 9699',getdate());</v>
       </c>
     </row>
@@ -4747,11 +4752,11 @@
         <v>405</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f>TEXT(F47,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1979-06-14</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'in@blandit.org','Maximiliano','Torres','374-989 Vivamus Av.','1979-06-14','16811108 1280',getdate());</v>
       </c>
     </row>
@@ -4778,11 +4783,11 @@
         <v>423</v>
       </c>
       <c r="H48" s="1" t="str">
-        <f>TEXT(F48,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1998-04-19</v>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ipsum.Curabitur.consequat@tinciduntDonec.org','Jeison','Tapia','Ap #482-3796 Pellentesque Rd.','1998-04-19','16070812 7543',getdate());</v>
       </c>
     </row>
@@ -4809,11 +4814,11 @@
         <v>18</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f>TEXT(F49,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1973-12-20</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ipsum.dolor.sit@sitametluctus.com','Vincent','Castro','Ap #442-543 Ultricies St.','1973-12-20','16670922 1136',getdate());</v>
       </c>
     </row>
@@ -4840,11 +4845,11 @@
         <v>343</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f>TEXT(F50,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1965-08-01</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ipsum.non@Donecelementumlorem.edu','Nikolas','Valdés','P.O. Box 100, 8127 Integer Av.','1965-08-01','16030207 3564',getdate());</v>
       </c>
     </row>
@@ -4871,11 +4876,11 @@
         <v>28</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f>TEXT(F51,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1997-01-27</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'lectus.a@Etiamligula.co.uk','Erick','Herrera','970-9830 Non Ave','1997-01-27','16641213 1358',getdate());</v>
       </c>
     </row>
@@ -4902,11 +4907,11 @@
         <v>211</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f>TEXT(F52,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1981-04-29</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ligula@convallis.net','Gerson','Pizarro','Ap #681-7407 Quisque St.','1981-04-29','16010413 2188',getdate());</v>
       </c>
     </row>
@@ -4933,11 +4938,11 @@
         <v>239</v>
       </c>
       <c r="H53" s="1" t="str">
-        <f>TEXT(F53,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1986-12-10</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ligula@dolor.org','Juliano','Pino','P.O. Box 104, 5002 Mauris St.','1986-12-10','16360919 9884',getdate());</v>
       </c>
     </row>
@@ -4964,11 +4969,11 @@
         <v>304</v>
       </c>
       <c r="H54" s="1" t="str">
-        <f>TEXT(F54,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1978-05-11</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'luctus.felis@lectusCumsociis.edu','Alberto','Contreras','603-5306 Id St.','1978-05-11','16081107 6777',getdate());</v>
       </c>
     </row>
@@ -4995,11 +5000,11 @@
         <v>418</v>
       </c>
       <c r="H55" s="1" t="str">
-        <f>TEXT(F55,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1973-09-26</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'luctus.ipsum.leo@ante.net','Gilberto','Godoy','4728 Mi Ave','1973-09-26','16071223 0432',getdate());</v>
       </c>
     </row>
@@ -5026,11 +5031,11 @@
         <v>109</v>
       </c>
       <c r="H56" s="1" t="str">
-        <f>TEXT(F56,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1982-03-19</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'malesuada.fames.ac@luctus.org','Randy','Ruiz','P.O. Box 835, 609 Risus Road','1982-03-19','16640320 7480',getdate());</v>
       </c>
     </row>
@@ -5057,11 +5062,11 @@
         <v>123</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f>TEXT(F57,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1991-11-17</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'massa.Vestibulum.accumsan@enim.co.uk','Pascual','Valenzuela','623-9098 Vitae St.','1991-11-17','16201108 8669',getdate());</v>
       </c>
     </row>
@@ -5088,11 +5093,11 @@
         <v>46</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f>TEXT(F58,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1969-12-21</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'mauris.Morbi.non@amet.ca','Christofer','Soto','Ap #720-2814 Nullam Avenue','1969-12-21','16781118 0038',getdate());</v>
       </c>
     </row>
@@ -5119,11 +5124,11 @@
         <v>258</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f>TEXT(F59,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1979-03-04</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'metus.In.nec@sollicitudinamalesuada.ca','Gerardo','Gutiérrez','P.O. Box 316, 7797 Fusce St.','1979-03-04','16000604 4739',getdate());</v>
       </c>
     </row>
@@ -5150,11 +5155,11 @@
         <v>104</v>
       </c>
       <c r="H60" s="1" t="str">
-        <f>TEXT(F60,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1975-02-18</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'mi@lorem.com','Teo','Hernández','9373 Risus Avenue','1975-02-18','16140120 1924',getdate());</v>
       </c>
     </row>
@@ -5181,11 +5186,11 @@
         <v>56</v>
       </c>
       <c r="H61" s="1" t="str">
-        <f>TEXT(F61,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1995-12-21</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'mollis@sedconsequat.org','Eduardo','Farías','8938 Risus. Ave','1995-12-21','16830318 6285',getdate());</v>
       </c>
     </row>
@@ -5212,11 +5217,11 @@
         <v>61</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f>TEXT(F62,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1980-09-27</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'mus.Proin.vel@Nunc.ca','Milovan','Jiménez','Ap #965-2713 Egestas. Road','1980-09-27','16641007 4311',getdate());</v>
       </c>
     </row>
@@ -5243,11 +5248,11 @@
         <v>167</v>
       </c>
       <c r="H63" s="1" t="str">
-        <f>TEXT(F63,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1999-10-09</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'neque.et.nunc@faucibus.net','Ander','Pérez','3450 Porttitor Av.','1999-10-09','16120725 5363',getdate());</v>
       </c>
     </row>
@@ -5274,11 +5279,11 @@
         <v>294</v>
       </c>
       <c r="H64" s="1" t="str">
-        <f>TEXT(F64,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1969-11-29</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'neque.In@lorem.co.uk','Yamir','Godoy','P.O. Box 374, 6573 Sed, Av.','1969-11-29','16260428 9203',getdate());</v>
       </c>
     </row>
@@ -5305,11 +5310,11 @@
         <v>234</v>
       </c>
       <c r="H65" s="1" t="str">
-        <f>TEXT(F65,"aaaa-mm-dd")</f>
+        <f t="shared" si="2"/>
         <v>1981-10-13</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'nisl.sem.consequat@blanditenim.ca','Franz','Torres','8609 Tempus Ave','1981-10-13','16521128 7452',getdate());</v>
       </c>
     </row>
@@ -5336,11 +5341,11 @@
         <v>442</v>
       </c>
       <c r="H66" s="1" t="str">
-        <f>TEXT(F66,"aaaa-mm-dd")</f>
+        <f t="shared" ref="H66:H101" si="3">TEXT(F66,"aaaa-mm-dd")</f>
         <v>1997-06-01</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'nisl.sem.consequat@idliberoDonec.org','Jhoan','González','Ap #637-4032 Proin St.','1997-06-01','16560515 1637',getdate());</v>
       </c>
     </row>
@@ -5367,11 +5372,11 @@
         <v>33</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f>TEXT(F67,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1989-11-27</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" ref="I67:I130" si="1">CONCATENATE("INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (",A67,", '",B67,"','",C67,"','",D67,"','",E67,"','",H67,"','",G67,"',getdate());")</f>
+        <f t="shared" ref="I67:I130" si="4">CONCATENATE("INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (",A67,", '",B67,"','",C67,"','",D67,"','",E67,"','",H67,"','",G67,"',getdate());")</f>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'nisl@lectus.com','Antwan','Alarcón','1773 Orci. St.','1989-11-27','16680908 7569',getdate());</v>
       </c>
     </row>
@@ -5398,11 +5403,11 @@
         <v>472</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f>TEXT(F68,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1984-09-22</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'non.quam.Pellentesque@ornareliberoat.com','Luckas','Jara','2560 Pede Road','1984-09-22','16580219 7854',getdate());</v>
       </c>
     </row>
@@ -5429,11 +5434,11 @@
         <v>114</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f>TEXT(F69,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1961-02-13</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Nulla.tempor.augue@tempus.org','Gilberto','Leiva','125-5418 Aenean Ave','1961-02-13','16200517 9615',getdate());</v>
       </c>
     </row>
@@ -5460,11 +5465,11 @@
         <v>51</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f>TEXT(F70,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1970-04-07</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'nunc.nulla.vulputate@lobortisnisi.org','Jairo','Molina','P.O. Box 762, 1055 Arcu. Avenue','1970-04-07','16900806 8596',getdate());</v>
       </c>
     </row>
@@ -5491,11 +5496,11 @@
         <v>428</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f>TEXT(F71,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1962-04-22</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'odio.auctor@interdumfeugiatSed.net','Yostin','Vera','200-1558 Malesuada St.','1962-04-22','16010219 8900',getdate());</v>
       </c>
     </row>
@@ -5522,11 +5527,11 @@
         <v>118</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f>TEXT(F72,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1978-08-29</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'odio.sagittis.semper@placerat.org','Isaak','Soto','875-2993 Morbi Rd.','1978-08-29','16000828 6163',getdate());</v>
       </c>
     </row>
@@ -5553,11 +5558,11 @@
         <v>95</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f>TEXT(F73,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1997-02-03</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'pede.Nunc@egetlacusMauris.net','Allan','Morales','202-6743 Pede Av.','1997-02-03','16460505 0691',getdate());</v>
       </c>
     </row>
@@ -5584,11 +5589,11 @@
         <v>467</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f>TEXT(F74,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1983-03-27</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Phasellus.nulla.Integer@Etiamgravidamolestie.net','Joakin','Soto','546-6455 Varius Ave','1983-03-27','16740322 0457',getdate());</v>
       </c>
     </row>
@@ -5615,11 +5620,11 @@
         <v>201</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f>TEXT(F75,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1970-04-11</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'placerat.Cras.dictum@Etiamvestibulum.org','Caleb','Martínez','170-443 Purus Rd.','1970-04-11','16270916 4038',getdate());</v>
       </c>
     </row>
@@ -5646,11 +5651,11 @@
         <v>410</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f>TEXT(F76,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1991-03-09</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'porttitor.interdum@Aliquamvulputateullamcorper.ca','Jesús','Salazar','Ap #246-4739 Nulla St.','1991-03-09','16300419 3888',getdate());</v>
       </c>
     </row>
@@ -5677,11 +5682,11 @@
         <v>285</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f>TEXT(F77,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1994-12-02</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'posuere.enim@atvelit.edu','Junior','Bustamante','Ap #915-1151 Sagittis Rd.','1994-12-02','16240724 6707',getdate());</v>
       </c>
     </row>
@@ -5708,11 +5713,11 @@
         <v>280</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f>TEXT(F78,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1988-09-01</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'purus.Maecenas.libero@ligulaelitpretium.com','Manuel','Cortés','392-142 At Avenue','1988-09-01','16470628 1674',getdate());</v>
       </c>
     </row>
@@ -5739,11 +5744,11 @@
         <v>243</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f>TEXT(F79,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1961-10-30</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'purus@magna.com','Henry','Parra','P.O. Box 630, 7037 Rutrum St.','1961-10-30','16660330 9573',getdate());</v>
       </c>
     </row>
@@ -5770,11 +5775,11 @@
         <v>455</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f>TEXT(F80,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1983-07-30</v>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Quisque.libero@justo.ca','Paulo','Sáez','P.O. Box 373, 4316 Id, Rd.','1983-07-30','16780920 6910',getdate());</v>
       </c>
     </row>
@@ -5801,11 +5806,11 @@
         <v>157</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f>TEXT(F81,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>2001-12-30</v>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'risus.Duis@eleifend.edu','Mirko','Cortés','Ap #349-5604 Fringilla, Road','2001-12-30','16990102 7152',getdate());</v>
       </c>
     </row>
@@ -5832,11 +5837,11 @@
         <v>175</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f>TEXT(F82,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1976-11-20</v>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'risus@nullaante.edu','George','Molina','P.O. Box 779, 7308 Quis Street','1976-11-20','16071211 9783',getdate());</v>
       </c>
     </row>
@@ -5863,11 +5868,11 @@
         <v>353</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f>TEXT(F83,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1966-02-12</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Sed.dictum@aceleifend.edu','Robin','Carvajal','408-9684 Id, Street','1966-02-12','16251010 2870',getdate());</v>
       </c>
     </row>
@@ -5894,11 +5899,11 @@
         <v>415</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f>TEXT(F84,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1967-11-24</v>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'sem.Nulla.interdum@cursus.com','Raul','Campos','186-5183 Ultrices Rd.','1967-11-24','16330203 0139',getdate());</v>
       </c>
     </row>
@@ -5925,11 +5930,11 @@
         <v>229</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f>TEXT(F85,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1980-02-07</v>
       </c>
       <c r="I85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'tempus.lorem@Quisqueornare.co.uk','Jorge','Alvarado','119-892 Magnis St.','1980-02-07','16331128 0329',getdate());</v>
       </c>
     </row>
@@ -5956,11 +5961,11 @@
         <v>450</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f>TEXT(F86,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1998-11-21</v>
       </c>
       <c r="I86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'tincidunt.congue.turpis@ametmassa.co.uk','Eddie','Paredes','3454 Elit, Road','1998-11-21','16561103 8000',getdate());</v>
       </c>
     </row>
@@ -5987,11 +5992,11 @@
         <v>71</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f>TEXT(F87,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1972-06-30</v>
       </c>
       <c r="I87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'tincidunt.congue@orciPhasellusdapibus.co.uk','Eydan','Vásquez','809-113 Nisi. Ave','1972-06-30','16800717 7564',getdate());</v>
       </c>
     </row>
@@ -6018,11 +6023,11 @@
         <v>333</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f>TEXT(F88,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1978-11-03</v>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'tincidunt@Sednullaante.ca','Ezekiel','Donoso','Ap #120-7266 Nibh. Avenue','1978-11-03','16360209 7366',getdate());</v>
       </c>
     </row>
@@ -6049,11 +6054,11 @@
         <v>85</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f>TEXT(F89,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1979-10-09</v>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'turpis.vitae@sedhendrerit.com','Yojhan','Lagos','2805 Facilisi. Rd.','1979-10-09','16030506 8710',getdate());</v>
       </c>
     </row>
@@ -6080,11 +6085,11 @@
         <v>152</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f>TEXT(F90,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1997-05-20</v>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ullamcorper.Duis@famesacturpis.org','Alexis','Moreno','Ap #971-9207 Lacus. Rd.','1997-05-20','16090101 3250',getdate());</v>
       </c>
     </row>
@@ -6111,11 +6116,11 @@
         <v>379</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f>TEXT(F91,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1985-09-22</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ullamcorper@pellentesquea.org','Danko','Castillo','Ap #693-7742 Faucibus. St.','1985-09-22','16940405 4315',getdate());</v>
       </c>
     </row>
@@ -6142,11 +6147,11 @@
         <v>224</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f>TEXT(F92,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1997-01-05</v>
       </c>
       <c r="I92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'ut.ipsum.ac@tellus.net','Daud','Silva','496-2397 Id, Avenue','1997-01-05','16091102 4263',getdate());</v>
       </c>
     </row>
@@ -6173,11 +6178,11 @@
         <v>138</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f>TEXT(F93,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>2001-12-16</v>
       </c>
       <c r="I93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Ut@aliquet.ca','Roberto','Salinas','Ap #239-755 Ipsum Street','2001-12-16','16891121 5328',getdate());</v>
       </c>
     </row>
@@ -6204,11 +6209,11 @@
         <v>248</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f>TEXT(F94,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1965-02-26</v>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'varius.et.euismod@dignissimlacusAliquam.com','Allen','Bustos','Ap #158-4641 Ac Rd.','1965-02-26','16121109 3917',getdate());</v>
       </c>
     </row>
@@ -6235,11 +6240,11 @@
         <v>267</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f>TEXT(F95,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1970-12-22</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'vel@euenim.com','Ian','Flores','P.O. Box 225, 7913 Sapien. St.','1970-12-22','16121116 0914',getdate());</v>
       </c>
     </row>
@@ -6266,11 +6271,11 @@
         <v>299</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f>TEXT(F96,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1979-01-21</v>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'Vestibulum@dictumProin.com','Tobías','Espinoza','P.O. Box 133, 5721 Consectetuer Rd.','1979-01-21','16510105 1364',getdate());</v>
       </c>
     </row>
@@ -6297,11 +6302,11 @@
         <v>445</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f>TEXT(F97,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1971-05-15</v>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'vitae.erat@eget.ca','Robin','Vargas','Ap #519-1280 Velit. Rd.','1971-05-15','16110313 2351',getdate());</v>
       </c>
     </row>
@@ -6328,11 +6333,11 @@
         <v>321</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f>TEXT(F98,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1976-10-01</v>
       </c>
       <c r="I98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'vitae.orci@acfacilisis.co.uk','Sandro','Torres','3987 Magna Ave','1976-10-01','16700715 3062',getdate());</v>
       </c>
     </row>
@@ -6359,11 +6364,11 @@
         <v>220</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f>TEXT(F99,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1961-02-26</v>
       </c>
       <c r="I99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'viverra@id.net','Damir','Ortega','276-5269 Vehicula Road','1961-02-26','16811002 3127',getdate());</v>
       </c>
     </row>
@@ -6390,11 +6395,11 @@
         <v>317</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f>TEXT(F100,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1999-09-29</v>
       </c>
       <c r="I100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'vulputate.nisi.sem@velarcueu.co.uk','Jahir','Herrera','531-7338 Euismod St.','1999-09-29','16521015 5973',getdate());</v>
       </c>
     </row>
@@ -6421,11 +6426,11 @@
         <v>193</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f>TEXT(F101,"aaaa-mm-dd")</f>
+        <f t="shared" si="3"/>
         <v>1985-04-06</v>
       </c>
       <c r="I101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (1, 'vulputate@Nullam.net','Mattia','Godoy','7661 Donec Rd.','1985-04-06','16890209 9798',getdate());</v>
       </c>
     </row>
@@ -6452,11 +6457,11 @@
         <v>478</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f t="shared" ref="H102:H165" si="2">TEXT(F102,"aaaa-mm-dd")</f>
+        <f t="shared" ref="H102:H165" si="5">TEXT(F102,"aaaa-mm-dd")</f>
         <v>1974-04-09</v>
       </c>
       <c r="I102" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'laoreet@tinciduntnunc.ca','Carolina','Orellana','P.O. Box 499, 3955 Sapien, Street','1974-04-09','16830124 1264',getdate());</v>
       </c>
     </row>
@@ -6483,11 +6488,11 @@
         <v>482</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1984-06-21</v>
       </c>
       <c r="I103" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'feugiat.Lorem.ipsum@aliquetlibero.net','Issidora','Vargas','Ap #169-4804 Quam, Ave','1984-06-21','16740407 7351',getdate());</v>
       </c>
     </row>
@@ -6514,11 +6519,11 @@
         <v>486</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1965-04-11</v>
       </c>
       <c r="I104" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'tellus.justo.sit@Duis.edu','Julia','Gutiérrez','P.O. Box 760, 5492 Diam. Street','1965-04-11','16430425 3331',getdate());</v>
       </c>
     </row>
@@ -6545,11 +6550,11 @@
         <v>490</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2001-01-21</v>
       </c>
       <c r="I105" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ipsum@leoelementumsem.ca','Alaniz','Salazar','Ap #410-4848 Sed Rd.','2001-01-21','16930811 5212',getdate());</v>
       </c>
     </row>
@@ -6576,11 +6581,11 @@
         <v>494</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1969-11-04</v>
       </c>
       <c r="I106" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'consequat.auctor.nunc@erat.ca','Jael','Orellana','8973 Dolor Street','1969-11-04','16331225 6385',getdate());</v>
       </c>
     </row>
@@ -6607,11 +6612,11 @@
         <v>498</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1999-12-31</v>
       </c>
       <c r="I107" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ante.ipsum.primis@dui.org','Helena','Olivares','Ap #276-4605 Ullamcorper Rd.','1999-12-31','16480812 7353',getdate());</v>
       </c>
     </row>
@@ -6638,11 +6643,11 @@
         <v>503</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1968-11-02</v>
       </c>
       <c r="I108" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'tincidunt.aliquam.arcu@mollisDuis.org','Amy','Aguilera','659-2718 Auctor Ave','1968-11-02','16830920 3670',getdate());</v>
       </c>
     </row>
@@ -6669,11 +6674,11 @@
         <v>507</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1996-05-28</v>
       </c>
       <c r="I109" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Sed.auctor.odio@magnamalesuadavel.ca','Skarleth','García','3724 Ante Rd.','1996-05-28','16240624 9488',getdate());</v>
       </c>
     </row>
@@ -6700,11 +6705,11 @@
         <v>512</v>
       </c>
       <c r="H110" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1992-11-16</v>
       </c>
       <c r="I110" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'scelerisque.dui.Suspendisse@ac.edu','Selena','Álvarez','6181 Urna. Rd.','1992-11-16','16470303 0082',getdate());</v>
       </c>
     </row>
@@ -6731,11 +6736,11 @@
         <v>516</v>
       </c>
       <c r="H111" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1993-01-15</v>
       </c>
       <c r="I111" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ultrices.iaculis@Vestibulumaccumsan.co.uk','Keyla','Sepúlveda','Ap #403-7885 Nulla Road','1993-01-15','16750206 8195',getdate());</v>
       </c>
     </row>
@@ -6762,11 +6767,11 @@
         <v>520</v>
       </c>
       <c r="H112" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1977-10-17</v>
       </c>
       <c r="I112" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Integer.sem@ornaresagittisfelis.org','Barbara','Gallardo','581-1791 Praesent Avenue','1977-10-17','16740916 7231',getdate());</v>
       </c>
     </row>
@@ -6793,11 +6798,11 @@
         <v>524</v>
       </c>
       <c r="H113" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1977-11-04</v>
       </c>
       <c r="I113" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'et.magnis@dapibusligula.ca','Nazareth','Martínez','788-778 A St.','1977-11-04','16981021 6813',getdate());</v>
       </c>
     </row>
@@ -6824,11 +6829,11 @@
         <v>528</v>
       </c>
       <c r="H114" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1990-09-28</v>
       </c>
       <c r="I114" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'risus.Duis@egestasAliquamnec.ca','Margarita','Peña','Ap #381-8935 Ipsum Rd.','1990-09-28','16840221 7619',getdate());</v>
       </c>
     </row>
@@ -6855,11 +6860,11 @@
         <v>532</v>
       </c>
       <c r="H115" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1998-08-21</v>
       </c>
       <c r="I115" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'semper.rutrum@justo.com','Sabina','Orellana','645-6385 Dui Road','1998-08-21','16241222 0333',getdate());</v>
       </c>
     </row>
@@ -6886,11 +6891,11 @@
         <v>536</v>
       </c>
       <c r="H116" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1964-05-19</v>
       </c>
       <c r="I116" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'vulputate@aliquetmetusurna.edu','Thais','Castro','Ap #575-6938 Cursus, Avenue','1964-05-19','16481204 8488',getdate());</v>
       </c>
     </row>
@@ -6917,11 +6922,11 @@
         <v>540</v>
       </c>
       <c r="H117" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1997-09-23</v>
       </c>
       <c r="I117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'erat.nonummy.ultricies@tellussemmollis.ca','Maylin','Venegas','Ap #890-1639 Ipsum Rd.','1997-09-23','16261020 2331',getdate());</v>
       </c>
     </row>
@@ -6948,11 +6953,11 @@
         <v>545</v>
       </c>
       <c r="H118" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1989-10-07</v>
       </c>
       <c r="I118" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'fames.ac@ridiculusmusProin.edu','Yanella','Díaz','8885 Enim. Avenue','1989-10-07','16750801 2833',getdate());</v>
       </c>
     </row>
@@ -6979,11 +6984,11 @@
         <v>549</v>
       </c>
       <c r="H119" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1986-11-24</v>
       </c>
       <c r="I119" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'In.condimentum@lobortisnisinibh.co.uk','Lidia','Farías','551-2515 Orci St.','1986-11-24','16340202 0923',getdate());</v>
       </c>
     </row>
@@ -7010,11 +7015,11 @@
         <v>554</v>
       </c>
       <c r="H120" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1965-06-02</v>
       </c>
       <c r="I120" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'parturient@Nullatempor.edu','Sharon','San Martín','8989 Dapibus Road','1965-06-02','16500510 1208',getdate());</v>
       </c>
     </row>
@@ -7041,11 +7046,11 @@
         <v>558</v>
       </c>
       <c r="H121" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1965-04-04</v>
       </c>
       <c r="I121" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'arcu.et.pede@dignissim.net','Ruth','Peña','965-6513 Nunc Av.','1965-04-04','16500121 7743',getdate());</v>
       </c>
     </row>
@@ -7072,11 +7077,11 @@
         <v>562</v>
       </c>
       <c r="H122" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1988-04-08</v>
       </c>
       <c r="I122" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'arcu@ultricies.ca','Rafaella','Espinoza','596-3031 Tempor Rd.','1988-04-08','16780102 0798',getdate());</v>
       </c>
     </row>
@@ -7103,11 +7108,11 @@
         <v>566</v>
       </c>
       <c r="H123" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1982-02-19</v>
       </c>
       <c r="I123" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'diam.vel@Donecvitaeerat.edu','Keily','Vargas','601-2904 Tincidunt. Rd.','1982-02-19','16140518 8135',getdate());</v>
       </c>
     </row>
@@ -7134,11 +7139,11 @@
         <v>570</v>
       </c>
       <c r="H124" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1960-07-09</v>
       </c>
       <c r="I124" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'felis@ipsum.org','Katrina','Castro','4535 Magna. St.','1960-07-09','16090630 4381',getdate());</v>
       </c>
     </row>
@@ -7165,11 +7170,11 @@
         <v>574</v>
       </c>
       <c r="H125" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1961-09-06</v>
       </c>
       <c r="I125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'sollicitudin.orci@SednequeSed.co.uk','Noemy','Vera','Ap #843-7830 Pellentesque. Rd.','1961-09-06','16900813 5650',getdate());</v>
       </c>
     </row>
@@ -7196,11 +7201,11 @@
         <v>578</v>
       </c>
       <c r="H126" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1995-08-26</v>
       </c>
       <c r="I126" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Integer.sem.elit@ridiculusmus.edu','Blanca','Bustamante','Ap #624-2277 In, Av.','1995-08-26','16210911 7131',getdate());</v>
       </c>
     </row>
@@ -7227,11 +7232,11 @@
         <v>582</v>
       </c>
       <c r="H127" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1991-07-24</v>
       </c>
       <c r="I127" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Duis.sit@non.org','Cristel','Toro','Ap #382-4570 Facilisis. Road','1991-07-24','16450726 7070',getdate());</v>
       </c>
     </row>
@@ -7258,11 +7263,11 @@
         <v>586</v>
       </c>
       <c r="H128" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1986-03-07</v>
       </c>
       <c r="I128" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ut.dolor@faucibus.com','Lorenza','Lagos','492-822 Eu Street','1986-03-07','16710208 9872',getdate());</v>
       </c>
     </row>
@@ -7289,11 +7294,11 @@
         <v>590</v>
       </c>
       <c r="H129" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1996-08-11</v>
       </c>
       <c r="I129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'risus.Donec.egestas@malesuadavel.edu','Marcia','Jiménez','Ap #484-9579 Eu St.','1996-08-11','16190301 0997',getdate());</v>
       </c>
     </row>
@@ -7320,11 +7325,11 @@
         <v>594</v>
       </c>
       <c r="H130" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2000-01-04</v>
       </c>
       <c r="I130" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'turpis.egestas.Fusce@ametluctus.ca','Rosa','Hernández','Ap #373-9167 Eget Avenue','2000-01-04','16010307 8614',getdate());</v>
       </c>
     </row>
@@ -7351,11 +7356,11 @@
         <v>598</v>
       </c>
       <c r="H131" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1990-06-10</v>
       </c>
       <c r="I131" t="str">
-        <f t="shared" ref="I131:I194" si="3">CONCATENATE("INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (",A131,", '",B131,"','",C131,"','",D131,"','",E131,"','",H131,"','",G131,"',getdate());")</f>
+        <f t="shared" ref="I131:I194" si="6">CONCATENATE("INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (",A131,", '",B131,"','",C131,"','",D131,"','",E131,"','",H131,"','",G131,"',getdate());")</f>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ullamcorper.Duis.cursus@penatibuset.org','Luz','Guzmán','455-201 Aliquam St.','1990-06-10','16640814 1874',getdate());</v>
       </c>
     </row>
@@ -7382,11 +7387,11 @@
         <v>603</v>
       </c>
       <c r="H132" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1997-04-15</v>
       </c>
       <c r="I132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'lorem@idmollis.com','Mercedes','Sánchez','7688 Semper Ave','1997-04-15','16280220 6322',getdate());</v>
       </c>
     </row>
@@ -7413,11 +7418,11 @@
         <v>607</v>
       </c>
       <c r="H133" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1995-08-01</v>
       </c>
       <c r="I133" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'magna@sagittisaugue.com','Dennise','Cáceres','410 Nunc Av.','1995-08-01','16640112 1543',getdate());</v>
       </c>
     </row>
@@ -7444,11 +7449,11 @@
         <v>612</v>
       </c>
       <c r="H134" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1987-05-21</v>
       </c>
       <c r="I134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Nullam.lobortis.quam@consectetueradipiscing.ca','Gisella','Rojas','214-2207 Donec St.','1987-05-21','16470625 3004',getdate());</v>
       </c>
     </row>
@@ -7475,11 +7480,11 @@
         <v>616</v>
       </c>
       <c r="H135" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1978-10-19</v>
       </c>
       <c r="I135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'sed.sem@et.edu','Piera','Olivares','P.O. Box 518, 3453 Metus St.','1978-10-19','16590410 2471',getdate());</v>
       </c>
     </row>
@@ -7506,11 +7511,11 @@
         <v>621</v>
       </c>
       <c r="H136" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1988-07-30</v>
       </c>
       <c r="I136" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'commodo.auctor@sodalespurusin.edu','Karen','Vega','Ap #853-3467 Et Avenue','1988-07-30','16810216 1604',getdate());</v>
       </c>
     </row>
@@ -7537,11 +7542,11 @@
         <v>625</v>
       </c>
       <c r="H137" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1994-10-30</v>
       </c>
       <c r="I137" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ac@asollicitudinorci.co.uk','Melody','Cárdenas','P.O. Box 686, 2953 Montes, Avenue','1994-10-30','16940206 2641',getdate());</v>
       </c>
     </row>
@@ -7568,11 +7573,11 @@
         <v>628</v>
       </c>
       <c r="H138" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1961-06-30</v>
       </c>
       <c r="I138" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'id.mollis.nec@vitaediamProin.net','Alaniz','Salazar','Ap #284-8152 Ante Rd.','1961-06-30','16380206 2079',getdate());</v>
       </c>
     </row>
@@ -7599,11 +7604,11 @@
         <v>632</v>
       </c>
       <c r="H139" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1964-07-04</v>
       </c>
       <c r="I139" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'fringilla.ornare@luctus.ca','Tabatha','Fernández','1569 Enim. Avenue','1964-07-04','16100504 9919',getdate());</v>
       </c>
     </row>
@@ -7630,11 +7635,11 @@
         <v>636</v>
       </c>
       <c r="H140" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1963-03-10</v>
       </c>
       <c r="I140" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'nunc.sed.pede@nequevenenatis.net','Sofía','Díaz','Ap #458-7056 Ultrices. Road','1963-03-10','16430608 4122',getdate());</v>
       </c>
     </row>
@@ -7661,11 +7666,11 @@
         <v>640</v>
       </c>
       <c r="H141" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1976-08-28</v>
       </c>
       <c r="I141" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'magna@pellentesqueafacilisis.co.uk','Amaya','Vera','P.O. Box 837, 9054 Lobortis St.','1976-08-28','16260511 1281',getdate());</v>
       </c>
     </row>
@@ -7692,11 +7697,11 @@
         <v>644</v>
       </c>
       <c r="H142" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2000-12-07</v>
       </c>
       <c r="I142" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'pellentesque@Donecelementum.org','Norma','González','P.O. Box 300, 1580 Augue Rd.','2000-12-07','16881130 6862',getdate());</v>
       </c>
     </row>
@@ -7723,11 +7728,11 @@
         <v>648</v>
       </c>
       <c r="H143" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1987-08-08</v>
       </c>
       <c r="I143" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'a.auctor.non@adipiscingnonluctus.org','Marthyna','Palma','P.O. Box 228, 5002 At, Rd.','1987-08-08','16220717 6534',getdate());</v>
       </c>
     </row>
@@ -7754,11 +7759,11 @@
         <v>651</v>
       </c>
       <c r="H144" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1972-09-03</v>
       </c>
       <c r="I144" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'tincidunt.nunc.ac@convallis.org','Karen','Pizarro','P.O. Box 824, 4306 Urna. Ave','1972-09-03','16960915 0033',getdate());</v>
       </c>
     </row>
@@ -7785,11 +7790,11 @@
         <v>655</v>
       </c>
       <c r="H145" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1966-12-23</v>
       </c>
       <c r="I145" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'augue.ac.ipsum@Quisqueornaretortor.edu','Karlita','Cáceres','3981 Neque. Avenue','1966-12-23','16281029 4625',getdate());</v>
       </c>
     </row>
@@ -7816,11 +7821,11 @@
         <v>659</v>
       </c>
       <c r="H146" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1961-07-30</v>
       </c>
       <c r="I146" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'mi.Aliquam.gravida@velitin.com','Marta','Vargas','P.O. Box 126, 7979 Diam Ave','1961-07-30','16330902 9084',getdate());</v>
       </c>
     </row>
@@ -7847,11 +7852,11 @@
         <v>664</v>
       </c>
       <c r="H147" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1970-05-20</v>
       </c>
       <c r="I147" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Quisque.fringilla@tinciduntaliquamarcu.org','Guadalupe','Sandoval','Ap #697-4544 Pharetra Street','1970-05-20','16190313 6651',getdate());</v>
       </c>
     </row>
@@ -7878,11 +7883,11 @@
         <v>668</v>
       </c>
       <c r="H148" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1964-12-04</v>
       </c>
       <c r="I148" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'lorem.luctus@porttitorerosnec.co.uk','Aynara','Donoso','453-2663 Enim, Rd.','1964-12-04','16691102 2538',getdate());</v>
       </c>
     </row>
@@ -7909,11 +7914,11 @@
         <v>672</v>
       </c>
       <c r="H149" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1988-05-12</v>
       </c>
       <c r="I149" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Nulla@placeratCrasdictum.ca','Emilia','Bravo','P.O. Box 115, 8195 Luctus Av.','1988-05-12','16581226 8281',getdate());</v>
       </c>
     </row>
@@ -7940,11 +7945,11 @@
         <v>675</v>
       </c>
       <c r="H150" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1981-01-21</v>
       </c>
       <c r="I150" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Quisque@mifringilla.ca','Karen','Molina','P.O. Box 440, 9750 Eget Ave','1981-01-21','16960418 6198',getdate());</v>
       </c>
     </row>
@@ -7971,11 +7976,11 @@
         <v>679</v>
       </c>
       <c r="H151" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1969-06-29</v>
       </c>
       <c r="I151" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'orci@ligulaconsectetuerrhoncus.net','Anahi','Alarcón','1118 Vitae, Rd.','1969-06-29','16880819 6961',getdate());</v>
       </c>
     </row>
@@ -8002,11 +8007,11 @@
         <v>683</v>
       </c>
       <c r="H152" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1985-09-29</v>
       </c>
       <c r="I152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'In@diamDuismi.ca','Francisca','Torres','4105 Aliquam Av.','1985-09-29','16000705 6708',getdate());</v>
       </c>
     </row>
@@ -8033,11 +8038,11 @@
         <v>687</v>
       </c>
       <c r="H153" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1993-05-07</v>
       </c>
       <c r="I153" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Nulla.dignissim@Duisami.com','Scarlette','Hernández','P.O. Box 365, 8312 Justo Street','1993-05-07','16240903 4291',getdate());</v>
       </c>
     </row>
@@ -8064,11 +8069,11 @@
         <v>691</v>
       </c>
       <c r="H154" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1965-04-08</v>
       </c>
       <c r="I154" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'eu.ligula.Aenean@fermentumarcuVestibulum.net','Dominic','Jiménez','Ap #429-7464 Dolor Street','1965-04-08','16551005 5105',getdate());</v>
       </c>
     </row>
@@ -8095,11 +8100,11 @@
         <v>695</v>
       </c>
       <c r="H155" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1982-07-09</v>
       </c>
       <c r="I155" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Maecenas@amet.edu','Milena','Herrera','Ap #585-2469 Sollicitudin St.','1982-07-09','16540805 6322',getdate());</v>
       </c>
     </row>
@@ -8126,11 +8131,11 @@
         <v>699</v>
       </c>
       <c r="H156" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1986-01-08</v>
       </c>
       <c r="I156" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'sit.amet@sociisnatoquepenatibus.org','Sarah','Vásquez','651-4345 Egestas. Rd.','1986-01-08','16561003 8985',getdate());</v>
       </c>
     </row>
@@ -8157,11 +8162,11 @@
         <v>702</v>
       </c>
       <c r="H157" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1996-05-17</v>
       </c>
       <c r="I157" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'feugiat.metus@arcuMorbi.edu','Dennise','Cárdenas','6632 Sodales Road','1996-05-17','16350701 0217',getdate());</v>
       </c>
     </row>
@@ -8188,11 +8193,11 @@
         <v>706</v>
       </c>
       <c r="H158" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1971-09-29</v>
       </c>
       <c r="I158" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ipsum.nunc@egetdictumplacerat.co.uk','Lauryn','Herrera','Ap #347-2538 Dignissim Street','1971-09-29','16371004 6362',getdate());</v>
       </c>
     </row>
@@ -8219,11 +8224,11 @@
         <v>710</v>
       </c>
       <c r="H159" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1997-10-01</v>
       </c>
       <c r="I159" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'erat.eget@interdumenim.ca','Charlotte','Olivares','P.O. Box 462, 2535 Rutrum, Avenue','1997-10-01','16680513 2666',getdate());</v>
       </c>
     </row>
@@ -8250,11 +8255,11 @@
         <v>714</v>
       </c>
       <c r="H160" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1984-10-01</v>
       </c>
       <c r="I160" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'mus.Proin@molestietellus.net','Nazareth','Henríquez','3269 Tempus St.','1984-10-01','16851117 3901',getdate());</v>
       </c>
     </row>
@@ -8281,11 +8286,11 @@
         <v>718</v>
       </c>
       <c r="H161" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1990-11-30</v>
       </c>
       <c r="I161" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ante@Proindolor.org','Genesis','Herrera','P.O. Box 504, 9922 At Rd.','1990-11-30','16470705 3056',getdate());</v>
       </c>
     </row>
@@ -8312,11 +8317,11 @@
         <v>722</v>
       </c>
       <c r="H162" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1993-10-12</v>
       </c>
       <c r="I162" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'bibendum@Fuscediam.ca','Kiara','Bravo','Ap #601-9242 Fusce Road','1993-10-12','16410829 4853',getdate());</v>
       </c>
     </row>
@@ -8343,11 +8348,11 @@
         <v>726</v>
       </c>
       <c r="H163" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1961-10-10</v>
       </c>
       <c r="I163" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'eget.tincidunt.dui@posuerecubiliaCurae.org','Mya','Pérez','868-7253 Vitae Rd.','1961-10-10','16590216 3780',getdate());</v>
       </c>
     </row>
@@ -8374,11 +8379,11 @@
         <v>730</v>
       </c>
       <c r="H164" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1966-12-30</v>
       </c>
       <c r="I164" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'nisl.arcu.iaculis@magnisdis.co.uk','Rebeca','Contreras','Ap #802-2481 In, Street','1966-12-30','16920420 8046',getdate());</v>
       </c>
     </row>
@@ -8405,11 +8410,11 @@
         <v>734</v>
       </c>
       <c r="H165" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1971-05-07</v>
       </c>
       <c r="I165" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'vitae@egestasrhoncus.ca','Dayra','Vera','161-7149 Vehicula Rd.','1971-05-07','16310418 0769',getdate());</v>
       </c>
     </row>
@@ -8436,11 +8441,11 @@
         <v>738</v>
       </c>
       <c r="H166" s="1" t="str">
-        <f t="shared" ref="H166:H201" si="4">TEXT(F166,"aaaa-mm-dd")</f>
+        <f t="shared" ref="H166:H201" si="7">TEXT(F166,"aaaa-mm-dd")</f>
         <v>1997-12-13</v>
       </c>
       <c r="I166" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ante.Maecenas.mi@magnaLorem.co.uk','Julieta','Martínez','Ap #673-9409 Nullam St.','1997-12-13','16440707 9724',getdate());</v>
       </c>
     </row>
@@ -8467,11 +8472,11 @@
         <v>742</v>
       </c>
       <c r="H167" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1971-02-01</v>
       </c>
       <c r="I167" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'felis@purusgravida.com','Anthonella','Rojas','8225 Curabitur Ave','1971-02-01','16020206 0398',getdate());</v>
       </c>
     </row>
@@ -8498,11 +8503,11 @@
         <v>746</v>
       </c>
       <c r="H168" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1961-09-27</v>
       </c>
       <c r="I168" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'leo@etmagnisdis.edu','Giselle','Contreras','Ap #295-4585 Elit Street','1961-09-27','16620615 5977',getdate());</v>
       </c>
     </row>
@@ -8529,11 +8534,11 @@
         <v>751</v>
       </c>
       <c r="H169" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1990-04-28</v>
       </c>
       <c r="I169" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Quisque.libero.lacus@auctorodio.org','Mariapaz','Sanhueza','P.O. Box 421, 7086 Porttitor Street','1990-04-28','16471216 4054',getdate());</v>
       </c>
     </row>
@@ -8560,11 +8565,11 @@
         <v>755</v>
       </c>
       <c r="H170" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2000-05-13</v>
       </c>
       <c r="I170" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'amet.ornare.lectus@pulvinararcuet.org','Makarena','Lagos','P.O. Box 304, 7790 Nulla Avenue','2000-05-13','16500402 2785',getdate());</v>
       </c>
     </row>
@@ -8591,11 +8596,11 @@
         <v>759</v>
       </c>
       <c r="H171" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1961-08-21</v>
       </c>
       <c r="I171" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'sed.sem.egestas@mollislectuspede.com','Tania','Lagos','Ap #993-3844 Scelerisque, Ave','1961-08-21','16590602 8906',getdate());</v>
       </c>
     </row>
@@ -8622,11 +8627,11 @@
         <v>763</v>
       </c>
       <c r="H172" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1999-07-26</v>
       </c>
       <c r="I172" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'fermentum.metus.Aenean@eratin.edu','Tabita','Bustos','820-6021 Duis Rd.','1999-07-26','16190201 7506',getdate());</v>
       </c>
     </row>
@@ -8653,11 +8658,11 @@
         <v>768</v>
       </c>
       <c r="H173" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1982-12-03</v>
       </c>
       <c r="I173" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'lobortis.tellus@enim.org','Pascalle','Muñoz','8978 Eleifend. Rd.','1982-12-03','16790429 3706',getdate());</v>
       </c>
     </row>
@@ -8684,11 +8689,11 @@
         <v>772</v>
       </c>
       <c r="H174" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1962-05-29</v>
       </c>
       <c r="I174" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'velit.eget.laoreet@sagittis.com','Betzabeth','Valenzuela','Ap #330-283 Penatibus Street','1962-05-29','16420811 1015',getdate());</v>
       </c>
     </row>
@@ -8715,11 +8720,11 @@
         <v>776</v>
       </c>
       <c r="H175" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1965-06-30</v>
       </c>
       <c r="I175" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Etiam.bibendum@Proin.ca','Priscila','Flores','P.O. Box 956, 7322 Dolor. St.','1965-06-30','16451021 3251',getdate());</v>
       </c>
     </row>
@@ -8746,11 +8751,11 @@
         <v>780</v>
       </c>
       <c r="H176" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2000-12-16</v>
       </c>
       <c r="I176" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'ultricies.ligula@sit.edu','Scarlet','Valdés','Ap #603-8693 Pede, Street','2000-12-16','16940804 1912',getdate());</v>
       </c>
     </row>
@@ -8777,11 +8782,11 @@
         <v>784</v>
       </c>
       <c r="H177" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1987-09-01</v>
       </c>
       <c r="I177" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'adipiscing.non.luctus@diamvelarcu.ca','Kathia','Soto','1430 Bibendum Street','1987-09-01','16260518 8164',getdate());</v>
       </c>
     </row>
@@ -8808,11 +8813,11 @@
         <v>788</v>
       </c>
       <c r="H178" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1991-08-02</v>
       </c>
       <c r="I178" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'justo@ipsumCurabiturconsequat.net','Escarleth','Sanhueza','Ap #370-1023 Vel, Rd.','1991-08-02','16770705 9957',getdate());</v>
       </c>
     </row>
@@ -8839,11 +8844,11 @@
         <v>792</v>
       </c>
       <c r="H179" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1985-06-10</v>
       </c>
       <c r="I179" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'eu@euerosNam.com','Elsa','Vidal','526-1006 Morbi St.','1985-06-10','16180426 1707',getdate());</v>
       </c>
     </row>
@@ -8870,11 +8875,11 @@
         <v>796</v>
       </c>
       <c r="H180" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1970-09-25</v>
       </c>
       <c r="I180" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'sed.sem.egestas@Nuncpulvinararcu.net','Jhendelyn','Cárdenas','4283 Dolor. Av.','1970-09-25','16541006 0502',getdate());</v>
       </c>
     </row>
@@ -8901,11 +8906,11 @@
         <v>799</v>
       </c>
       <c r="H181" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1965-01-16</v>
       </c>
       <c r="I181" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'adipiscing.enim@neceleifendnon.edu','Tania','Rojas','Ap #541-8484 Duis Road','1965-01-16','16920722 7761',getdate());</v>
       </c>
     </row>
@@ -8932,11 +8937,11 @@
         <v>803</v>
       </c>
       <c r="H182" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1975-12-01</v>
       </c>
       <c r="I182" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'enim@sed.com','Naomy','Álvarez','Ap #565-8302 Praesent Street','1975-12-01','16640915 1625',getdate());</v>
       </c>
     </row>
@@ -8963,11 +8968,11 @@
         <v>807</v>
       </c>
       <c r="H183" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2000-02-29</v>
       </c>
       <c r="I183" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'pharetra.nibh@rhoncusProinnisl.org','Susan','González','557-4796 Eleifend, Av.','2000-02-29','16610528 4464',getdate());</v>
       </c>
     </row>
@@ -8994,11 +8999,11 @@
         <v>811</v>
       </c>
       <c r="H184" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1984-06-03</v>
       </c>
       <c r="I184" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'tempor.lorem.eget@fringilla.ca','Amaral','González','5581 Arcu. Rd.','1984-06-03','16240621 3385',getdate());</v>
       </c>
     </row>
@@ -9025,11 +9030,11 @@
         <v>815</v>
       </c>
       <c r="H185" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1989-09-24</v>
       </c>
       <c r="I185" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'luctus.et.ultrices@ametconsectetuer.com','Jasmine','Leiva','Ap #747-3724 Morbi Street','1989-09-24','16781012 0480',getdate());</v>
       </c>
     </row>
@@ -9056,11 +9061,11 @@
         <v>819</v>
       </c>
       <c r="H186" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1995-11-10</v>
       </c>
       <c r="I186" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Praesent@molestietellusAenean.co.uk','Elisabet','Gallardo','Ap #101-4384 Nibh. Av.','1995-11-10','16540826 9784',getdate());</v>
       </c>
     </row>
@@ -9087,11 +9092,11 @@
         <v>823</v>
       </c>
       <c r="H187" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1987-04-15</v>
       </c>
       <c r="I187" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Nulla.eget@apurus.org','Anita','Díaz','P.O. Box 889, 6902 Est. Street','1987-04-15','16490710 6498',getdate());</v>
       </c>
     </row>
@@ -9118,11 +9123,11 @@
         <v>827</v>
       </c>
       <c r="H188" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1971-11-22</v>
       </c>
       <c r="I188" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'sed@est.net','Viviana','Bustamante','Ap #611-5704 Dui. St.','1971-11-22','16480828 4964',getdate());</v>
       </c>
     </row>
@@ -9149,11 +9154,11 @@
         <v>831</v>
       </c>
       <c r="H189" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1978-04-11</v>
       </c>
       <c r="I189" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Morbi.metus@Nam.org','Madeleine','Vidal','2127 Vivamus Avenue','1978-04-11','16410712 2329',getdate());</v>
       </c>
     </row>
@@ -9180,11 +9185,11 @@
         <v>835</v>
       </c>
       <c r="H190" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1961-01-12</v>
       </c>
       <c r="I190" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'at@Aliquamerat.org','Masiel','Fernández','Ap #663-9837 Mi Street','1961-01-12','16781128 7296',getdate());</v>
       </c>
     </row>
@@ -9211,11 +9216,11 @@
         <v>839</v>
       </c>
       <c r="H191" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1968-01-30</v>
       </c>
       <c r="I191" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Cras.convallis.convallis@ut.net','Andrea','Poblete','Ap #710-6634 Cras Rd.','1968-01-30','16061115 4014',getdate());</v>
       </c>
     </row>
@@ -9242,11 +9247,11 @@
         <v>843</v>
       </c>
       <c r="H192" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1964-01-19</v>
       </c>
       <c r="I192" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'mauris@Namnulla.ca','Simoney','Araya','P.O. Box 151, 4696 Tempus St.','1964-01-19','16201027 4807',getdate());</v>
       </c>
     </row>
@@ -9273,11 +9278,11 @@
         <v>847</v>
       </c>
       <c r="H193" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1986-06-11</v>
       </c>
       <c r="I193" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'Maecenas.malesuada.fringilla@pretiumaliquet.co.uk','Marian','Carrasco','Ap #163-3566 Auctor Avenue','1986-06-11','16701204 9941',getdate());</v>
       </c>
     </row>
@@ -9304,11 +9309,11 @@
         <v>851</v>
       </c>
       <c r="H194" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1982-05-03</v>
       </c>
       <c r="I194" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'mus.Proin.vel@Cras.co.uk','Claudia','Torres','P.O. Box 198, 3967 Turpis. Road','1982-05-03','16570103 4315',getdate());</v>
       </c>
     </row>
@@ -9335,11 +9340,11 @@
         <v>855</v>
       </c>
       <c r="H195" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1968-05-25</v>
       </c>
       <c r="I195" t="str">
-        <f t="shared" ref="I195:I201" si="5">CONCATENATE("INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (",A195,", '",B195,"','",C195,"','",D195,"','",E195,"','",H195,"','",G195,"',getdate());")</f>
+        <f t="shared" ref="I195:I201" si="8">CONCATENATE("INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (",A195,", '",B195,"','",C195,"','",D195,"','",E195,"','",H195,"','",G195,"',getdate());")</f>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'consequat@risus.net','Elena','Sáez','4976 Fringilla Road','1968-05-25','16631126 6453',getdate());</v>
       </c>
     </row>
@@ -9366,11 +9371,11 @@
         <v>859</v>
       </c>
       <c r="H196" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1961-01-15</v>
       </c>
       <c r="I196" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'congue.elit.sed@nonummyutmolestie.net','Noemí','Soto','542-130 Odio Ave','1961-01-15','16450714 8478',getdate());</v>
       </c>
     </row>
@@ -9397,11 +9402,11 @@
         <v>863</v>
       </c>
       <c r="H197" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1969-05-30</v>
       </c>
       <c r="I197" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'amet@CurabiturdictumPhasellus.org','Siomara','Gómez','3481 Dictum St.','1969-05-30','16720428 9008',getdate());</v>
       </c>
     </row>
@@ -9428,11 +9433,11 @@
         <v>867</v>
       </c>
       <c r="H198" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1971-03-05</v>
       </c>
       <c r="I198" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'sapien@nibhenim.co.uk','Tonka','Carrasco','573-1180 Aliquet Rd.','1971-03-05','16400904 2765',getdate());</v>
       </c>
     </row>
@@ -9459,11 +9464,11 @@
         <v>871</v>
       </c>
       <c r="H199" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1963-05-19</v>
       </c>
       <c r="I199" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'et.libero.Proin@Nulla.co.uk','Isidora','Vera','Ap #244-8073 Mi Road','1963-05-19','16171018 6410',getdate());</v>
       </c>
     </row>
@@ -9490,11 +9495,11 @@
         <v>875</v>
       </c>
       <c r="H200" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1964-07-01</v>
       </c>
       <c r="I200" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'gravida.Aliquam.tincidunt@sedsemegestas.net','Denisse','Martínez','Ap #396-5863 Cursus Ave','1964-07-01','16180907 4527',getdate());</v>
       </c>
     </row>
@@ -9521,11 +9526,11 @@
         <v>879</v>
       </c>
       <c r="H201" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1997-10-01</v>
       </c>
       <c r="I201" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>INSERT INTO [dbo].[Customer] (GenderId,Email,FirstName,LastName,Address,BirthDate,PhoneNumber,CreationDate)  VALUES (2, 'quis.diam@ultricesmauris.net','Maria','Soto','4276 Non, Ave','1997-10-01','16170405 2735',getdate());</v>
       </c>
     </row>
@@ -9743,7 +9748,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'LG K40S 32 GB aurora black 2 GB RAM',1);</v>
       </c>
     </row>
-    <row r="21" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D21" s="6" t="s">
         <v>907</v>
       </c>
@@ -9752,7 +9757,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'LG K50S 32 GB aurora black 3 GB RAM',1);</v>
       </c>
     </row>
-    <row r="22" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D22" s="6" t="s">
         <v>908</v>
       </c>
@@ -9770,7 +9775,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'MÁS VENDIDO',1);</v>
       </c>
     </row>
-    <row r="24" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D24" s="6" t="s">
         <v>910</v>
       </c>
@@ -9779,7 +9784,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Moto E6 Play 32 GB negro 2 GB RAM',1);</v>
       </c>
     </row>
-    <row r="25" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D25" s="6" t="s">
         <v>911</v>
       </c>
@@ -9788,7 +9793,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Moto E6 Plus 32 GB bright cherry 2 GB RAM',1);</v>
       </c>
     </row>
-    <row r="26" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D26" s="6" t="s">
         <v>912</v>
       </c>
@@ -9797,7 +9802,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Moto E6s (2020) 32 GB gravity gradient 2 GB RAM',1);</v>
       </c>
     </row>
-    <row r="27" spans="4:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:6" ht="72" x14ac:dyDescent="0.3">
       <c r="D27" s="6" t="s">
         <v>913</v>
       </c>
@@ -9806,7 +9811,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Moto E6s (2020) Special Edition 64 GB gravity gradient 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="28" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D28" s="6" t="s">
         <v>914</v>
       </c>
@@ -9815,7 +9820,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Moto G8 Plus 64 GB cosmic blue 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="29" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D29" s="6" t="s">
         <v>915</v>
       </c>
@@ -9824,7 +9829,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Moto G8 Power 64 GB vulcan 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="30" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D30" s="6" t="s">
         <v>916</v>
       </c>
@@ -9833,7 +9838,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Moto G8 Power Lite 64 GB turquesa 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="31" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D31" s="6" t="s">
         <v>917</v>
       </c>
@@ -9842,7 +9847,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Moto G9 Play 64 GB rosa spring 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="32" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D32" s="6" t="s">
         <v>918</v>
       </c>
@@ -9851,7 +9856,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Motorola Edge 128 GB rojo plum 6 GB RAM',1);</v>
       </c>
     </row>
-    <row r="33" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D33" s="6" t="s">
         <v>919</v>
       </c>
@@ -9860,7 +9865,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Motorola Edge Special Edition 256 GB rojo plum 6 GB RAM',1);</v>
       </c>
     </row>
-    <row r="34" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D34" s="6" t="s">
         <v>920</v>
       </c>
@@ -9869,7 +9874,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Motorola One Fusion 128 GB emerald green 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="35" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D35" s="6" t="s">
         <v>921</v>
       </c>
@@ -9878,7 +9883,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Motorola One Hyper 128 GB deepsea blue 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="36" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D36" s="6" t="s">
         <v>922</v>
       </c>
@@ -9887,7 +9892,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Motorola One Macro 64 GB space blue 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="37" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D37" s="6" t="s">
         <v>923</v>
       </c>
@@ -9896,7 +9901,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A01 32 GB azul 2 GB RAM',1);</v>
       </c>
     </row>
-    <row r="38" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D38" s="6" t="s">
         <v>924</v>
       </c>
@@ -9905,7 +9910,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A01 Core 16 GB negro 1 GB RAM',1);</v>
       </c>
     </row>
-    <row r="39" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D39" s="6" t="s">
         <v>925</v>
       </c>
@@ -9914,7 +9919,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A10 32 GB negro 2 GB RAM',1);</v>
       </c>
     </row>
-    <row r="40" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D40" s="6" t="s">
         <v>926</v>
       </c>
@@ -9923,7 +9928,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A10s 32 GB azul 2 GB RAM',1);</v>
       </c>
     </row>
-    <row r="41" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D41" s="6" t="s">
         <v>927</v>
       </c>
@@ -9932,7 +9937,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A11 64 GB negro 3 GB RAM',1);</v>
       </c>
     </row>
-    <row r="42" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D42" s="6" t="s">
         <v>928</v>
       </c>
@@ -9941,7 +9946,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A20s 32 GB negro 3 GB RAM',1);</v>
       </c>
     </row>
-    <row r="43" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D43" s="6" t="s">
         <v>929</v>
       </c>
@@ -9950,7 +9955,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A21s 64 GB blanco 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="44" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D44" s="6" t="s">
         <v>930</v>
       </c>
@@ -9959,7 +9964,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A30s 64 GB prism crush black 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="45" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D45" s="6" t="s">
         <v>931</v>
       </c>
@@ -9968,7 +9973,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A31 128 GB prism crush blue 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="46" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D46" s="6" t="s">
         <v>932</v>
       </c>
@@ -9977,7 +9982,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A51 128 GB prism crush black 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="47" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D47" s="6" t="s">
         <v>933</v>
       </c>
@@ -9986,7 +9991,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy A71 128 GB prism crush silver 6 GB RAM',1);</v>
       </c>
     </row>
-    <row r="48" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D48" s="6" t="s">
         <v>934</v>
       </c>
@@ -9995,7 +10000,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy J2 Core 16 GB negro 1 GB RAM',1);</v>
       </c>
     </row>
-    <row r="49" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D49" s="6" t="s">
         <v>935</v>
       </c>
@@ -10004,7 +10009,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy Note20 256 GB bronce místico 8 GB RAM',1);</v>
       </c>
     </row>
-    <row r="50" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D50" s="6" t="s">
         <v>936</v>
       </c>
@@ -10013,7 +10018,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy S10 128 GB negro prisma 8 GB RAM',1);</v>
       </c>
     </row>
-    <row r="51" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D51" s="6" t="s">
         <v>937</v>
       </c>
@@ -10022,7 +10027,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy S20 128 GB cosmic gray 8 GB RAM',1);</v>
       </c>
     </row>
-    <row r="52" spans="4:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D52" s="6" t="s">
         <v>938</v>
       </c>
@@ -10031,7 +10036,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Samsung Galaxy S20+ 128 GB cloud blue 8 GB RAM',1);</v>
       </c>
     </row>
-    <row r="53" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D53" s="6" t="s">
         <v>939</v>
       </c>
@@ -10040,7 +10045,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Xiaomi Redmi 9 Dual SIM 32 GB carbon grey 3 GB RAM',1);</v>
       </c>
     </row>
-    <row r="54" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:6" ht="72" x14ac:dyDescent="0.3">
       <c r="D54" s="6" t="s">
         <v>940</v>
       </c>
@@ -10049,7 +10054,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Xiaomi Redmi 9A Dual SIM 32 GB verde majestuoso 2 GB RAM',1);</v>
       </c>
     </row>
-    <row r="55" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D55" s="6" t="s">
         <v>941</v>
       </c>
@@ -10058,7 +10063,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Xiaomi Redmi Note 8 Dual SIM 64 GB Space black 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="56" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:6" ht="72" x14ac:dyDescent="0.3">
       <c r="D56" s="6" t="s">
         <v>942</v>
       </c>
@@ -10067,7 +10072,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Xiaomi Redmi Note 8 Pro Dual SIM 64 GB gris mineral 6 GB RAM',1);</v>
       </c>
     </row>
-    <row r="57" spans="4:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:6" ht="72" x14ac:dyDescent="0.3">
       <c r="D57" s="6" t="s">
         <v>943</v>
       </c>
@@ -10076,7 +10081,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Xiaomi Redmi Note 9 Dual SIM 128 GB verde bosque 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="58" spans="4:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="D58" s="6" t="s">
         <v>944</v>
       </c>
@@ -10085,7 +10090,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Xiaomi Redmi Note 9 Pro (64 Mpx) Dual SIM 64 GB gris interestelar 6 GB RAM',1);</v>
       </c>
     </row>
-    <row r="59" spans="4:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:6" ht="72" x14ac:dyDescent="0.3">
       <c r="D59" s="6" t="s">
         <v>945</v>
       </c>
@@ -10094,7 +10099,7 @@
         <v>INSERT INTO [dbo].[Product] VALUES (ROUND(RAND()*1000000000,0),'Xiaomi Redmi Note 9S Dual SIM 64 GB gris interestelar 4 GB RAM',1);</v>
       </c>
     </row>
-    <row r="60" spans="4:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D60" s="6" t="s">
         <v>946</v>
       </c>
@@ -10179,7 +10184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F39E809-7C30-4EF5-BA12-407043747143}">
   <dimension ref="C4:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -10256,4 +10261,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4312745D-FC80-4B39-A2BA-BF28524578F0}">
+  <dimension ref="C4:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>952</v>
+      </c>
+      <c r="D4" s="9">
+        <v>48340</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="9">
+        <v>386656</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="9">
+        <v>397356</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="9">
+        <v>159708</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="9">
+        <v>255244</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="9">
+        <v>241396</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f>SUM(D4:D9)</f>
+        <v>1488700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>